<commit_message>
[102]-Update dashboard - Cuong
</commit_message>
<xml_diff>
--- a/assets/public/csv/export/Loans.xlsx
+++ b/assets/public/csv/export/Loans.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="45">
   <si>
     <t>ĐẠI HỌC HUẾ</t>
   </si>
@@ -609,7 +609,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O92"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="G16" sqref="G16"/>
@@ -994,765 +994,808 @@
         <v>29</v>
       </c>
     </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="28">
+        <v>45407.33507755787</v>
+      </c>
+      <c r="E19" s="28">
+        <v>45415</v>
+      </c>
+      <c r="G19" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D20" s="28">
-        <v>45407.33507755787</v>
+        <v>45407.337384467595</v>
       </c>
       <c r="E20" s="28">
-        <v>45415</v>
+        <v>45408</v>
       </c>
       <c r="G20" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="28">
+        <v>45407.33758047454</v>
+      </c>
+      <c r="F21" s="28">
+        <v>45407.33758047454</v>
+      </c>
+      <c r="G21" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
         <v>28</v>
       </c>
       <c r="D22" s="28">
-        <v>45407.337384467595</v>
+        <v>45407.36531197917</v>
       </c>
       <c r="E22" s="28">
-        <v>45408</v>
+        <v>45407</v>
       </c>
       <c r="G22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="28">
+        <v>45407.370896759254</v>
+      </c>
+      <c r="E23" s="28">
+        <v>45407</v>
+      </c>
+      <c r="G23" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
         <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D24" s="28">
-        <v>45407.33758047454</v>
+        <v>45407.371061134254</v>
       </c>
       <c r="F24" s="28">
-        <v>45407.33758047454</v>
+        <v>45407.371061134254</v>
       </c>
       <c r="G24" t="s">
         <v>33</v>
       </c>
     </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="28">
+        <v>45407.37112768518</v>
+      </c>
+      <c r="E25" s="28">
+        <v>45415</v>
+      </c>
+      <c r="G25" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C26" t="s">
         <v>28</v>
       </c>
       <c r="D26" s="28">
-        <v>45407.36531197917</v>
-      </c>
-      <c r="E26" s="28">
-        <v>45407</v>
+        <v>45407.37128040509</v>
+      </c>
+      <c r="F26" s="28">
+        <v>45407.37128040509</v>
       </c>
       <c r="G26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="28">
+        <v>45407.37259475695</v>
+      </c>
+      <c r="E27" s="28">
+        <v>45408</v>
+      </c>
+      <c r="G27" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B28" t="s">
         <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D28" s="28">
-        <v>45407.370896759254</v>
-      </c>
-      <c r="E28" s="28">
+        <v>45407.37294758102</v>
+      </c>
+      <c r="F28" s="28">
+        <v>45407.37294758102</v>
+      </c>
+      <c r="G28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="28">
+        <v>45407.37682925926</v>
+      </c>
+      <c r="E29" s="28">
         <v>45407</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G29" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D30" s="28">
-        <v>45407.371061134254</v>
-      </c>
-      <c r="F30" s="28">
-        <v>45407.371061134254</v>
+        <v>45407.37696179398</v>
+      </c>
+      <c r="E30" s="28">
+        <v>45403</v>
       </c>
       <c r="G30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="28">
+        <v>45407.37717476852</v>
+      </c>
+      <c r="F31" s="28">
+        <v>45407.37717476852</v>
+      </c>
+      <c r="G31" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D32" s="28">
-        <v>45407.37112768518</v>
+        <v>45407.37736916667</v>
       </c>
       <c r="E32" s="28">
-        <v>45415</v>
+        <v>45407</v>
       </c>
       <c r="G32" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>16</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="28">
+        <v>45407.37795408565</v>
+      </c>
+      <c r="F33" s="28">
+        <v>45407.37795408565</v>
+      </c>
+      <c r="G33" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D34" s="28">
-        <v>45407.37128040509</v>
-      </c>
-      <c r="F34" s="28">
-        <v>45407.37128040509</v>
+        <v>45407.378153240745</v>
+      </c>
+      <c r="E34" s="28">
+        <v>45421</v>
       </c>
       <c r="G34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>18</v>
+      </c>
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" s="28">
+        <v>45407.3784390625</v>
+      </c>
+      <c r="F35" s="28">
+        <v>45407.3784390625</v>
+      </c>
+      <c r="G35" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D36" s="28">
-        <v>45407.37259475695</v>
-      </c>
-      <c r="E36" s="28">
-        <v>45408</v>
+        <v>45407.37946521991</v>
+      </c>
+      <c r="F36" s="28">
+        <v>45407.37946521991</v>
       </c>
       <c r="G36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>20</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" s="28">
+        <v>45407.38039980324</v>
+      </c>
+      <c r="E37" s="28">
+        <v>45409</v>
+      </c>
+      <c r="G37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B38" t="s">
         <v>32</v>
       </c>
       <c r="C38" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D38" s="28">
-        <v>45407.37294758102</v>
-      </c>
-      <c r="F38" s="28">
-        <v>45407.37294758102</v>
+        <v>45407.3805468287</v>
+      </c>
+      <c r="E38" s="28">
+        <v>45423</v>
       </c>
       <c r="G38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>22</v>
+      </c>
+      <c r="B39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" s="28">
+        <v>45407.381407361114</v>
+      </c>
+      <c r="F39" s="28">
+        <v>45407.381407361114</v>
+      </c>
+      <c r="G39" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C40" t="s">
         <v>36</v>
       </c>
       <c r="D40" s="28">
-        <v>45407.37682925926</v>
-      </c>
-      <c r="E40" s="28">
-        <v>45407</v>
+        <v>45407.38298628472</v>
+      </c>
+      <c r="F40" s="28">
+        <v>45407.38298628472</v>
       </c>
       <c r="G40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>24</v>
+      </c>
+      <c r="B41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" s="28">
+        <v>45407.38437539352</v>
+      </c>
+      <c r="E41" s="28">
+        <v>45424</v>
+      </c>
+      <c r="G41" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B42" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C42" t="s">
         <v>36</v>
       </c>
       <c r="D42" s="28">
-        <v>45407.37696179398</v>
+        <v>45407.38577636574</v>
       </c>
       <c r="E42" s="28">
-        <v>45403</v>
+        <v>45424</v>
+      </c>
+      <c r="F42" s="28">
+        <v>45407.38577636574</v>
       </c>
       <c r="G42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>26</v>
+      </c>
+      <c r="B43" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" s="28">
+        <v>45407.39798105324</v>
+      </c>
+      <c r="E43" s="28">
+        <v>45408</v>
+      </c>
+      <c r="G43" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D44" s="28">
-        <v>45407.37717476852</v>
+        <v>45407.399041655095</v>
+      </c>
+      <c r="E44" s="28">
+        <v>45408</v>
       </c>
       <c r="F44" s="28">
-        <v>45407.37717476852</v>
+        <v>45407.399041655095</v>
       </c>
       <c r="G44" t="s">
         <v>33</v>
       </c>
     </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>28</v>
+      </c>
+      <c r="B45" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45" t="s">
+        <v>31</v>
+      </c>
+      <c r="D45" s="28">
+        <v>45407.40624190972</v>
+      </c>
+      <c r="E45" s="28">
+        <v>45415</v>
+      </c>
+      <c r="F45" s="28">
+        <v>45407.40624190972</v>
+      </c>
+      <c r="G45" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C46" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D46" s="28">
-        <v>45407.37736916667</v>
+        <v>45407.42877266204</v>
       </c>
       <c r="E46" s="28">
-        <v>45407</v>
+        <v>45408</v>
       </c>
       <c r="G46" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>30</v>
+      </c>
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="28">
+        <v>45407.42940736111</v>
+      </c>
+      <c r="E47" s="28">
+        <v>45408</v>
+      </c>
+      <c r="F47" s="28">
+        <v>45407.42940736111</v>
+      </c>
+      <c r="G47" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B48" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C48" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D48" s="28">
-        <v>45407.37795408565</v>
-      </c>
-      <c r="F48" s="28">
-        <v>45407.37795408565</v>
+        <v>45407.57074332176</v>
+      </c>
+      <c r="E48" s="28">
+        <v>45409</v>
       </c>
       <c r="G48" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>32</v>
+      </c>
+      <c r="B49" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" t="s">
+        <v>31</v>
+      </c>
+      <c r="D49" s="28">
+        <v>45407.5708703125</v>
+      </c>
+      <c r="E49" s="28">
+        <v>45404</v>
+      </c>
+      <c r="G49" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B50" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D50" s="28">
-        <v>45407.378153240745</v>
+        <v>45407.571015532405</v>
       </c>
       <c r="E50" s="28">
-        <v>45421</v>
+        <v>45416</v>
       </c>
       <c r="G50" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>34</v>
+      </c>
+      <c r="B51" t="s">
+        <v>37</v>
+      </c>
+      <c r="C51" t="s">
+        <v>31</v>
+      </c>
+      <c r="D51" s="28">
+        <v>45407.57874349537</v>
+      </c>
+      <c r="E51" s="28">
+        <v>45401</v>
+      </c>
+      <c r="G51" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C52" t="s">
+        <v>44</v>
+      </c>
+      <c r="D52" s="28">
+        <v>45408.10591292824</v>
+      </c>
+      <c r="E52" s="28">
+        <v>45412</v>
+      </c>
+      <c r="G52" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53">
         <v>36</v>
       </c>
-      <c r="D52" s="28">
-        <v>45407.3784390625</v>
-      </c>
-      <c r="F52" s="28">
-        <v>45407.3784390625</v>
-      </c>
-      <c r="G52" t="s">
+      <c r="B53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C53" t="s">
+        <v>44</v>
+      </c>
+      <c r="D53" s="28">
+        <v>45408.10667378472</v>
+      </c>
+      <c r="E53" s="28">
+        <v>45412</v>
+      </c>
+      <c r="F53" s="28">
+        <v>45408.10667378472</v>
+      </c>
+      <c r="G53" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B54" t="s">
         <v>37</v>
       </c>
       <c r="C54" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D54" s="28">
-        <v>45407.37946521991</v>
+        <v>45408.66402711805</v>
+      </c>
+      <c r="E54" s="28">
+        <v>45401</v>
       </c>
       <c r="F54" s="28">
-        <v>45407.37946521991</v>
+        <v>45408.66402711805</v>
       </c>
       <c r="G54" t="s">
         <v>33</v>
       </c>
     </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>38</v>
+      </c>
+      <c r="B55" t="s">
+        <v>42</v>
+      </c>
+      <c r="C55" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" s="28">
+        <v>45408.67029363426</v>
+      </c>
+      <c r="E55" s="28">
+        <v>45416</v>
+      </c>
+      <c r="F55" s="28">
+        <v>45408.67029363426</v>
+      </c>
+      <c r="G55" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B56" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C56" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D56" s="28">
-        <v>45407.38039980324</v>
+        <v>45410.161463564815</v>
       </c>
       <c r="E56" s="28">
         <v>45409</v>
       </c>
+      <c r="F56" s="28">
+        <v>45410.161463564815</v>
+      </c>
       <c r="G56" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>21</v>
-      </c>
-      <c r="B58" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58" t="s">
-        <v>36</v>
-      </c>
-      <c r="D58" s="28">
-        <v>45407.3805468287</v>
-      </c>
-      <c r="E58" s="28">
-        <v>45423</v>
-      </c>
-      <c r="G58" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>22</v>
-      </c>
-      <c r="B60" t="s">
-        <v>38</v>
-      </c>
-      <c r="C60" t="s">
-        <v>36</v>
-      </c>
-      <c r="D60" s="28">
-        <v>45407.381407361114</v>
-      </c>
-      <c r="F60" s="28">
-        <v>45407.381407361114</v>
-      </c>
-      <c r="G60" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>23</v>
-      </c>
-      <c r="B62" t="s">
-        <v>32</v>
-      </c>
-      <c r="C62" t="s">
-        <v>36</v>
-      </c>
-      <c r="D62" s="28">
-        <v>45407.38298628472</v>
-      </c>
-      <c r="F62" s="28">
-        <v>45407.38298628472</v>
-      </c>
-      <c r="G62" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>24</v>
-      </c>
-      <c r="B64" t="s">
-        <v>32</v>
-      </c>
-      <c r="C64" t="s">
-        <v>36</v>
-      </c>
-      <c r="D64" s="28">
-        <v>45407.38437539352</v>
-      </c>
-      <c r="E64" s="28">
-        <v>45424</v>
-      </c>
-      <c r="G64" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>25</v>
-      </c>
-      <c r="B66" t="s">
-        <v>32</v>
-      </c>
-      <c r="C66" t="s">
-        <v>36</v>
-      </c>
-      <c r="D66" s="28">
-        <v>45407.38577636574</v>
-      </c>
-      <c r="E66" s="28">
-        <v>45424</v>
-      </c>
-      <c r="F66" s="28">
-        <v>45407.38577636574</v>
-      </c>
-      <c r="G66" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>26</v>
-      </c>
-      <c r="B68" t="s">
-        <v>39</v>
-      </c>
-      <c r="C68" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>40</v>
+      </c>
+      <c r="B57" t="s">
+        <v>40</v>
+      </c>
+      <c r="C57" t="s">
         <v>31</v>
       </c>
-      <c r="D68" s="28">
-        <v>45407.39798105324</v>
-      </c>
-      <c r="E68" s="28">
-        <v>45408</v>
-      </c>
-      <c r="G68" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>27</v>
-      </c>
-      <c r="B70" t="s">
-        <v>39</v>
-      </c>
-      <c r="C70" t="s">
-        <v>31</v>
-      </c>
-      <c r="D70" s="28">
-        <v>45407.399041655095</v>
-      </c>
-      <c r="E70" s="28">
-        <v>45408</v>
-      </c>
-      <c r="F70" s="28">
-        <v>45407.399041655095</v>
-      </c>
-      <c r="G70" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>28</v>
-      </c>
-      <c r="B72" t="s">
-        <v>30</v>
-      </c>
-      <c r="C72" t="s">
-        <v>31</v>
-      </c>
-      <c r="D72" s="28">
-        <v>45407.40624190972</v>
-      </c>
-      <c r="E72" s="28">
-        <v>45415</v>
-      </c>
-      <c r="F72" s="28">
-        <v>45407.40624190972</v>
-      </c>
-      <c r="G72" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>29</v>
-      </c>
-      <c r="B74" t="s">
-        <v>30</v>
-      </c>
-      <c r="C74" t="s">
-        <v>31</v>
-      </c>
-      <c r="D74" s="28">
-        <v>45407.42877266204</v>
-      </c>
-      <c r="E74" s="28">
-        <v>45408</v>
-      </c>
-      <c r="G74" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>30</v>
-      </c>
-      <c r="B76" t="s">
-        <v>30</v>
-      </c>
-      <c r="C76" t="s">
-        <v>31</v>
-      </c>
-      <c r="D76" s="28">
-        <v>45407.42940736111</v>
-      </c>
-      <c r="E76" s="28">
-        <v>45408</v>
-      </c>
-      <c r="F76" s="28">
-        <v>45407.42940736111</v>
-      </c>
-      <c r="G76" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>31</v>
-      </c>
-      <c r="B78" t="s">
-        <v>40</v>
-      </c>
-      <c r="C78" t="s">
-        <v>31</v>
-      </c>
-      <c r="D78" s="28">
-        <v>45407.57074332176</v>
-      </c>
-      <c r="E78" s="28">
-        <v>45409</v>
-      </c>
-      <c r="G78" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>32</v>
-      </c>
-      <c r="B80" t="s">
-        <v>41</v>
-      </c>
-      <c r="C80" t="s">
-        <v>31</v>
-      </c>
-      <c r="D80" s="28">
-        <v>45407.5708703125</v>
-      </c>
-      <c r="E80" s="28">
-        <v>45404</v>
-      </c>
-      <c r="G80" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>33</v>
-      </c>
-      <c r="B82" t="s">
-        <v>42</v>
-      </c>
-      <c r="C82" t="s">
-        <v>31</v>
-      </c>
-      <c r="D82" s="28">
-        <v>45407.571015532405</v>
-      </c>
-      <c r="E82" s="28">
-        <v>45416</v>
-      </c>
-      <c r="G82" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>34</v>
-      </c>
-      <c r="B84" t="s">
-        <v>37</v>
-      </c>
-      <c r="C84" t="s">
-        <v>31</v>
-      </c>
-      <c r="D84" s="28">
-        <v>45407.57874349537</v>
-      </c>
-      <c r="E84" s="28">
-        <v>45401</v>
-      </c>
-      <c r="G84" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>35</v>
-      </c>
-      <c r="B86" t="s">
-        <v>43</v>
-      </c>
-      <c r="C86" t="s">
-        <v>44</v>
-      </c>
-      <c r="D86" s="28">
-        <v>45408.10591292824</v>
-      </c>
-      <c r="E86" s="28">
-        <v>45412</v>
-      </c>
-      <c r="G86" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>36</v>
-      </c>
-      <c r="B88" t="s">
-        <v>43</v>
-      </c>
-      <c r="C88" t="s">
-        <v>44</v>
-      </c>
-      <c r="D88" s="28">
-        <v>45408.10667378472</v>
-      </c>
-      <c r="E88" s="28">
-        <v>45412</v>
-      </c>
-      <c r="F88" s="28">
-        <v>45408.10667378472</v>
-      </c>
-      <c r="G88" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>37</v>
-      </c>
-      <c r="B90" t="s">
-        <v>37</v>
-      </c>
-      <c r="C90" t="s">
-        <v>31</v>
-      </c>
-      <c r="D90" s="28">
-        <v>45408.66402711805</v>
-      </c>
-      <c r="E90" s="28">
-        <v>45401</v>
-      </c>
-      <c r="F90" s="28">
-        <v>45408.66402711805</v>
-      </c>
-      <c r="G90" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>38</v>
-      </c>
-      <c r="B92" t="s">
-        <v>42</v>
-      </c>
-      <c r="C92" t="s">
-        <v>31</v>
-      </c>
-      <c r="D92" s="28">
-        <v>45408.67029363426</v>
-      </c>
-      <c r="E92" s="28">
-        <v>45416</v>
-      </c>
-      <c r="F92" s="28">
-        <v>45408.67029363426</v>
-      </c>
-      <c r="G92" t="s">
-        <v>33</v>
+      <c r="D57" s="28">
+        <v>45410.16192521991</v>
+      </c>
+      <c r="E57" s="28">
+        <v>45411</v>
+      </c>
+      <c r="G57" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>